<commit_message>
AD3-456 Microdata table sorting not correct
</commit_message>
<xml_diff>
--- a/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/agricWomenDataset-Template.xlsx
+++ b/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/agricWomenDataset-Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -331,10 +331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,462 +420,238 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>